<commit_message>
Update excel file by adding quotation marks
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables.xlsx
+++ b/JupyterNotebooks/variables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018C3824-01D4-4ADA-B56E-00093B152FB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4415542-ED9B-4259-A27F-E300582959F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,15 +43,9 @@
     <t>OtherAlg2: [Cryptomonad]</t>
   </si>
   <si>
-    <t>PMax</t>
-  </si>
-  <si>
     <t>Inner Variable Name</t>
   </si>
   <si>
-    <t>KPO4</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>Maximum photosynthetic rate</t>
+  </si>
+  <si>
+    <t>"PMax"</t>
+  </si>
+  <si>
+    <t>"KPO4"</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -405,7 +405,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -422,13 +422,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -439,13 +439,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update variables and the produced input file
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/variables.xlsx
+++ b/JupyterNotebooks/variables.xlsx
@@ -3,24 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4415542-ED9B-4259-A27F-E300582959F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243662AD-EC7D-401F-BF3E-C434F4CA950B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plants" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -31,9 +36,15 @@
     <t>Variable Name</t>
   </si>
   <si>
+    <t>Inner Variable Name</t>
+  </si>
+  <si>
     <t>Tune</t>
   </si>
   <si>
+    <t>Initial Value</t>
+  </si>
+  <si>
     <t>Estimated sensetivity</t>
   </si>
   <si>
@@ -43,7 +54,10 @@
     <t>OtherAlg2: [Cryptomonad]</t>
   </si>
   <si>
-    <t>Inner Variable Name</t>
+    <t>Maximum photosynthetic rate</t>
+  </si>
+  <si>
+    <t>"PMax"</t>
   </si>
   <si>
     <t>yes</t>
@@ -52,13 +66,25 @@
     <t>Concentration of P in water needed for 50 % of maximum intake</t>
   </si>
   <si>
-    <t>Maximum photosynthetic rate</t>
-  </si>
-  <si>
-    <t>"PMax"</t>
-  </si>
-  <si>
     <t>"KPO4"</t>
+  </si>
+  <si>
+    <t>Exponential factor for suboptimal conditions</t>
+  </si>
+  <si>
+    <t>"EMort"</t>
+  </si>
+  <si>
+    <t>Minimum light saturation</t>
+  </si>
+  <si>
+    <t>"MinLightSat"</t>
+  </si>
+  <si>
+    <t>Slope or rate of change per 10°C temperature change (maybe photosynthesis?)</t>
+  </si>
+  <si>
+    <t>"TempRespSlope"</t>
   </si>
 </sst>
 </file>
@@ -379,22 +405,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.05078125" customWidth="1"/>
-    <col min="2" max="3" width="25.89453125" customWidth="1"/>
-    <col min="4" max="4" width="17.7890625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="19.26171875" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,47 +431,116 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>3.9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>